<commit_message>
adjusted excel according to new multiLanguage-object
</commit_message>
<xml_diff>
--- a/multilanguage.xlsx
+++ b/multilanguage.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="18060" windowHeight="8835"/>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="LIST_LANG">tables!$A$1:$A$2</definedName>
-    <definedName name="SELECT_LANG">multilanguage!$B$2</definedName>
+    <definedName name="SELECT_LANG">multilanguage!$A$2</definedName>
     <definedName name="TABLE_LANGID">tables!$A$1:$B$2</definedName>
     <definedName name="TABLE_TRANSLATION">multilanguage!$B$6:$D$19</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>var</t>
   </si>
@@ -35,18 +35,9 @@
     <t>select language:</t>
   </si>
   <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
     <t>Zurücksetzen</t>
   </si>
   <si>
-    <t>SELECT</t>
-  </si>
-  <si>
     <t>Auswählen</t>
   </si>
   <si>
@@ -56,12 +47,6 @@
     <t>Character</t>
   </si>
   <si>
-    <t>CHAR</t>
-  </si>
-  <si>
-    <t>TALK</t>
-  </si>
-  <si>
     <t>Sprechen</t>
   </si>
   <si>
@@ -74,9 +59,6 @@
     <t>Reset</t>
   </si>
   <si>
-    <t>THINK</t>
-  </si>
-  <si>
     <t>Denken</t>
   </si>
   <si>
@@ -86,42 +68,21 @@
     <t>OOC</t>
   </si>
   <si>
-    <t>ROLL</t>
-  </si>
-  <si>
     <t>Würfeln</t>
   </si>
   <si>
     <t>Roll</t>
   </si>
   <si>
-    <t>INSERT</t>
-  </si>
-  <si>
     <t>Einfügen</t>
   </si>
   <si>
     <t>Insert</t>
   </si>
   <si>
-    <t>ROLL_title</t>
-  </si>
-  <si>
-    <t>OOC_title</t>
-  </si>
-  <si>
-    <t>TALK_title</t>
-  </si>
-  <si>
-    <t>THINK_title</t>
-  </si>
-  <si>
     <t>Out Of Character</t>
   </si>
   <si>
-    <t>CHAR_title</t>
-  </si>
-  <si>
     <t>Name des Charakters</t>
   </si>
   <si>
@@ -132,6 +93,51 @@
   </si>
   <si>
     <t>Posting Tool fürs Forenspiel (Play by Post)</t>
+  </si>
+  <si>
+    <t>Translation (paste this in the code)</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>talk_title</t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>think_title</t>
+  </si>
+  <si>
+    <t>ooc</t>
+  </si>
+  <si>
+    <t>ooc_title</t>
+  </si>
+  <si>
+    <t>roll</t>
+  </si>
+  <si>
+    <t>roll_title</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>character_title</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +180,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -198,22 +210,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -227,7 +369,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="0000FF"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -512,258 +654,260 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="str">
         <f>"// MULTILANGUAGE: "&amp;SELECT_LANG</f>
         <v>// MULTILANGUAGE: English</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="str">
-        <f t="shared" ref="A6:A19" si="0">"ml" &amp;B6 &amp;"='" &amp;VLOOKUP(B6, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
-        <v>mlTITLE='Posting Tool for Forum-PbP (Play by Post)';</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B6 &amp;"='" &amp;VLOOKUP(B6, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.title='Posting Tool for Forum-PbP (Play by Post)';</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B7 &amp;"='" &amp;VLOOKUP(B7, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.reset='Reset';</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B8 &amp;"='" &amp;VLOOKUP(B8, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.select='Select';</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B9 &amp;"='" &amp;VLOOKUP(B9, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.talk='Talk';</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B10 &amp;"='" &amp;VLOOKUP(B10, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.talk_title='Talk';</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B11 &amp;"='" &amp;VLOOKUP(B11, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.think='Think';</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B12 &amp;"='" &amp;VLOOKUP(B12, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.think_title='Think';</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B13 &amp;"='" &amp;VLOOKUP(B13, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.ooc='OOC';</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B14 &amp;"='" &amp;VLOOKUP(B14, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.ooc_title='Out Of Character';</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B15 &amp;"='" &amp;VLOOKUP(B15, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.roll='Roll';</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B16 &amp;"='" &amp;VLOOKUP(B16, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.roll_title='Roll';</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B17 &amp;"='" &amp;VLOOKUP(B17, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.insert='Insert';</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlRESET='Reset';</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B18 &amp;"='" &amp;VLOOKUP(B18, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.character='Character';</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlSELECT='Select';</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlTALK='Talk';</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlTALK_title='Talk';</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlTHINK='Think';</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlTHINK_title='Think';</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlOOC='OOC';</v>
-      </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>"postingTool.multiLanguage.strings." &amp;B19 &amp;"='" &amp;VLOOKUP(B19, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
+        <v>postingTool.multiLanguage.strings.character_title='Name of character';</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlOOC_title='Out Of Character';</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlROLL='Roll';</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D19" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlROLL_title='Roll';</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlINSERT='Insert';</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="str">
-        <f t="shared" ref="A18" si="1">"ml" &amp;B18 &amp;"='" &amp;VLOOKUP(B18, TABLE_TRANSLATION, VLOOKUP(SELECT_LANG, TABLE_LANGID, 2, FALSE), FALSE)&amp;"';"</f>
-        <v>mlCHAR='Character';</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>mlCHAR_title='Name of character';</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:D5 B2 A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:D5 A2:A3">
       <formula1>LIST_LANG</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>